<commit_message>
Doc Update - final before revision
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ufo12\FAV\Bachelor\Bachelor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3490B96-AA39-49E9-B748-152091C99897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E70719-456F-4B75-B219-89476BAC118E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -416,6 +416,43 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -458,10 +495,10 @@
     <xf numFmtId="21" fontId="1" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="1" fillId="6" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1"/>
-    <xf numFmtId="21" fontId="1" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="1" fillId="5" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="1" fillId="5" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="3" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="1" fillId="5" borderId="19" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="1" fillId="5" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="1" fillId="5" borderId="21" xfId="4" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20 % – Zvýraznění 1" xfId="3" builtinId="30"/>
@@ -749,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E6" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +821,7 @@
         <f t="shared" ref="D3:E3" si="0">D9-D8</f>
         <v>1.5810185185185177E-2</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="29">
         <f t="shared" si="0"/>
         <v>4.4664351851851913E-2</v>
       </c>
@@ -801,7 +838,7 @@
         <f t="shared" ref="D4:E4" si="1">D11-D10</f>
         <v>1.5578703703703622E-2</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="30">
         <f t="shared" si="1"/>
         <v>4.5486111111111116E-2</v>
       </c>
@@ -818,7 +855,7 @@
         <f t="shared" ref="D5:E5" si="2">D13-D12</f>
         <v>1.4884259259259291E-2</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="30">
         <f t="shared" si="2"/>
         <v>4.5104166666666723E-2</v>
       </c>
@@ -835,8 +872,8 @@
         <f t="shared" ref="D6:E6" si="3">AVERAGE(D3:D5)</f>
         <v>1.5424382716049364E-2</v>
       </c>
-      <c r="E6" s="30">
-        <f t="shared" si="3"/>
+      <c r="E6" s="31">
+        <f>AVERAGE(E3:E5)</f>
         <v>4.5084876543209917E-2</v>
       </c>
     </row>
@@ -921,7 +958,7 @@
       <c r="D13" s="14">
         <v>0.77577546296296296</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="28">
         <v>0.96549768518518519</v>
       </c>
     </row>

</xml_diff>